<commit_message>
Add Referees and Corner Men to spreadsheet
</commit_message>
<xml_diff>
--- a/TitleBoutII.xlsx
+++ b/TitleBoutII.xlsx
@@ -8,9 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Boxing Action Cards" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Heavyweights" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="KD-KO Table" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Cards" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Referees" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Corner Men" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Heavyweights" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="KD-KO Table" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="215">
   <si>
     <t xml:space="preserve">CF</t>
   </si>
@@ -103,6 +105,402 @@
   </si>
   <si>
     <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fouls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stoppage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consistency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boxer Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elmo Adolph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julio Alvarado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rudy Battle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very Lenient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Late</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenny Bayless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert Byrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Early</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frank Cappuccino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stanley Christodoulou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lawrence Cole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lenient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joe Cortez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eddie Cotton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joey Curtis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marty Denkin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arthur Donovan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vic Draculich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benjy Esteves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lou Filippo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roy Francis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armando Garcia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruby Goldstein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mitch Halpern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larry Hazzard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wayne Kelly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mills Lane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arthur Mercante Jr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arthur Mercante Sr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Octavio Meyran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russell Mora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lou Moret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jay Nady</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Randy Neumann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John O’Brien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terry O’Connor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlos Padilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dave Parris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Davey Pearl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tony Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jack Reiss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isidro Rodriguez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larry Rozadilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pat Russell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frank Sikora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">George Siler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steve Smoger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richard Steele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harold Valan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jersey Joe Walcott</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waldemar Schmidt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tony Weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel Van de Wiele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuts/Swell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eddie Aliano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excellent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ray Arcel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very Good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teddy Atlas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nacho Beristain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dan Birmingham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jack Blackburn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chuck Bodak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pete Brodsky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommy Brooks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freddie Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ralph Citro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gil Clancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pepe Correa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cus D’Amato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jimmy DeForrest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miguel Diaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yancey Durham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lou Duva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlos Espada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chick Ferrara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouie Fisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danny Florio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nick Floria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eddie Fuch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joe Gallagher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert Garcia Cortez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al Gavin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richie Giachetti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlie Goldman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virgil Hunter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brendan Ingle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John David Jackson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Izzy Klein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenny Lane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peter Manfredo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floyd Mayweather Sr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shane McGuigan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ace Moratta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rudy Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesse Reid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eddy Reynoso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazim Richardson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freddie Roach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hector Roca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin Rooney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dick Sadler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abel Sanchez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luis Sarria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manny Seamon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ronnie Shields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al Silvani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aaron Snowell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sam Solomon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joe Souza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emanuel Steward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don Turner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victor Vallee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mick Williamson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom Yankello</t>
   </si>
   <si>
     <t xml:space="preserve">Nickname</t>
@@ -378,7 +776,7 @@
   <dimension ref="A1:N101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A102" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A102" activeCellId="0" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4857,10 +5255,2494 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F51"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.77"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="E47" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="E49" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="E50" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="E51" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G61"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G61" activeCellId="0" sqref="G61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="10.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.77"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AY1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4911,154 +7793,154 @@
         <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>161</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>30</v>
+        <v>162</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>163</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>32</v>
+        <v>164</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>35</v>
+        <v>167</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>36</v>
+        <v>168</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>37</v>
+        <v>169</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>38</v>
+        <v>170</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>39</v>
+        <v>171</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>40</v>
+        <v>172</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>41</v>
+        <v>173</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>42</v>
+        <v>174</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>43</v>
+        <v>175</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>45</v>
+        <v>177</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>46</v>
+        <v>178</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>49</v>
+        <v>181</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>50</v>
+        <v>182</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>51</v>
+        <v>183</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>53</v>
+        <v>185</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>54</v>
+        <v>186</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>55</v>
+        <v>187</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>56</v>
+        <v>188</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>57</v>
+        <v>189</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>59</v>
+        <v>191</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>60</v>
+        <v>192</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>61</v>
+        <v>193</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>62</v>
+        <v>194</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>63</v>
+        <v>195</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>64</v>
+        <v>196</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>65</v>
+        <v>197</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>66</v>
+        <v>198</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>67</v>
+        <v>199</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>68</v>
+        <v>200</v>
       </c>
       <c r="AR1" s="2" t="s">
-        <v>69</v>
+        <v>201</v>
       </c>
       <c r="AS1" s="2" t="s">
-        <v>70</v>
+        <v>202</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>71</v>
+        <v>203</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>72</v>
+        <v>204</v>
       </c>
       <c r="AV1" s="2" t="s">
-        <v>73</v>
+        <v>205</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>74</v>
+        <v>206</v>
       </c>
       <c r="AX1" s="2" t="s">
-        <v>75</v>
+        <v>207</v>
       </c>
       <c r="AY1" s="2" t="s">
-        <v>76</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -5072,820 +7954,820 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="3" style="0" width="6.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="3" style="1" width="6.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="n">
+      <c r="A1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="n">
+      <c r="D1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="n">
+      <c r="E1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="0" t="n">
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I1" s="0" t="n">
+      <c r="I1" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="J1" s="0" t="n">
+      <c r="J1" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="K1" s="0" t="n">
+      <c r="K1" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="L1" s="0" t="n">
+      <c r="L1" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="L2" s="0" t="n">
+      <c r="B2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L2" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L3" s="0" t="n">
+      <c r="B3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L4" s="0" t="n">
+      <c r="B4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="L4" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L5" s="0" t="n">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="L5" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L6" s="0" t="n">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="L6" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>78</v>
+      <c r="B7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>78</v>
+      <c r="B8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>79</v>
+      <c r="B9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>79</v>
+      <c r="B10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>80</v>
+      <c r="B11" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>80</v>
+      <c r="B12" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>81</v>
+      <c r="B13" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>81</v>
+      <c r="B14" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>81</v>
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="L16" s="0" t="s">
-        <v>81</v>
+      <c r="B16" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>81</v>
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>81</v>
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>81</v>
+      <c r="B19" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="L20" s="0" t="s">
-        <v>81</v>
+      <c r="B20" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>81</v>
+      <c r="B21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>